<commit_message>
fixing the bug with position
</commit_message>
<xml_diff>
--- a/application/data/Generated ReportEmployee_Allowance_Auditing_Result_Report.xlsx
+++ b/application/data/Generated ReportEmployee_Allowance_Auditing_Result_Report.xlsx
@@ -27,19 +27,13 @@
     <sheet name="Jul-2022CommHighPosition" sheetId="18" r:id="rId18"/>
     <sheet name="Jul-2022CommNormal" sheetId="19" r:id="rId19"/>
     <sheet name="Jul-2022InvalidCommAllow" sheetId="20" r:id="rId20"/>
-    <sheet name="Nov-2022CarTransportAllowance" sheetId="21" r:id="rId21"/>
-    <sheet name="Nov-2022noGradeWithAllowance" sheetId="22" r:id="rId22"/>
-    <sheet name="Nov-2022noStatusWithAllowance" sheetId="23" r:id="rId23"/>
-    <sheet name="Nov-2022CarAllowNot60" sheetId="24" r:id="rId24"/>
-    <sheet name="Nov-2022CommNormal" sheetId="25" r:id="rId25"/>
-    <sheet name="Nov-2022InvalidCommAllow" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4360" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4218" uniqueCount="378">
   <si>
     <t>CPR_NO</t>
   </si>
@@ -1173,12 +1167,6 @@
   </si>
   <si>
     <t>P3-STEP 2</t>
-  </si>
-  <si>
-    <t>_</t>
-  </si>
-  <si>
-    <t>HOUSING_ALLOW</t>
   </si>
 </sst>
 </file>
@@ -17292,2526 +17280,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>622</v>
-      </c>
-      <c r="D2">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>622</v>
-      </c>
-      <c r="D4">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>622</v>
-      </c>
-      <c r="D6">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>378</v>
-      </c>
-      <c r="C8">
-        <v>622</v>
-      </c>
-      <c r="D8">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>378</v>
-      </c>
-      <c r="C9">
-        <v>12</v>
-      </c>
-      <c r="D9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>622</v>
-      </c>
-      <c r="D10">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>378</v>
-      </c>
-      <c r="C12">
-        <v>622</v>
-      </c>
-      <c r="D12">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>378</v>
-      </c>
-      <c r="C13">
-        <v>12</v>
-      </c>
-      <c r="D13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>622</v>
-      </c>
-      <c r="D14">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>12</v>
-      </c>
-      <c r="D15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>378</v>
-      </c>
-      <c r="C16">
-        <v>622</v>
-      </c>
-      <c r="D16">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>378</v>
-      </c>
-      <c r="C17">
-        <v>12</v>
-      </c>
-      <c r="D17">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>622</v>
-      </c>
-      <c r="D18">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>12</v>
-      </c>
-      <c r="D19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>378</v>
-      </c>
-      <c r="C20">
-        <v>622</v>
-      </c>
-      <c r="D20">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>378</v>
-      </c>
-      <c r="C21">
-        <v>12</v>
-      </c>
-      <c r="D21">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J41"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>810</v>
-      </c>
-      <c r="E2">
-        <v>800</v>
-      </c>
-      <c r="F2">
-        <v>3020</v>
-      </c>
-      <c r="G2">
-        <v>622</v>
-      </c>
-      <c r="H2">
-        <v>1200</v>
-      </c>
-      <c r="I2">
-        <v>630</v>
-      </c>
-      <c r="J2">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>13</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>13</v>
-      </c>
-      <c r="G3">
-        <v>12</v>
-      </c>
-      <c r="H3">
-        <v>72</v>
-      </c>
-      <c r="I3">
-        <v>12</v>
-      </c>
-      <c r="J3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
-      </c>
-      <c r="E4">
-        <v>44</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>25</v>
-      </c>
-      <c r="J4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>50</v>
-      </c>
-      <c r="E5">
-        <v>44</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>25</v>
-      </c>
-      <c r="J5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>810</v>
-      </c>
-      <c r="E6">
-        <v>800</v>
-      </c>
-      <c r="F6">
-        <v>3020</v>
-      </c>
-      <c r="G6">
-        <v>622</v>
-      </c>
-      <c r="H6">
-        <v>1200</v>
-      </c>
-      <c r="I6">
-        <v>630</v>
-      </c>
-      <c r="J6">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>13</v>
-      </c>
-      <c r="E7">
-        <v>10</v>
-      </c>
-      <c r="F7">
-        <v>13</v>
-      </c>
-      <c r="G7">
-        <v>12</v>
-      </c>
-      <c r="H7">
-        <v>72</v>
-      </c>
-      <c r="I7">
-        <v>12</v>
-      </c>
-      <c r="J7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>50</v>
-      </c>
-      <c r="E8">
-        <v>44</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>25</v>
-      </c>
-      <c r="J8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>50</v>
-      </c>
-      <c r="E9">
-        <v>44</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>25</v>
-      </c>
-      <c r="J9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>810</v>
-      </c>
-      <c r="E10">
-        <v>800</v>
-      </c>
-      <c r="F10">
-        <v>3020</v>
-      </c>
-      <c r="G10">
-        <v>622</v>
-      </c>
-      <c r="H10">
-        <v>1200</v>
-      </c>
-      <c r="I10">
-        <v>630</v>
-      </c>
-      <c r="J10">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>13</v>
-      </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="F11">
-        <v>13</v>
-      </c>
-      <c r="G11">
-        <v>12</v>
-      </c>
-      <c r="H11">
-        <v>72</v>
-      </c>
-      <c r="I11">
-        <v>12</v>
-      </c>
-      <c r="J11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>50</v>
-      </c>
-      <c r="E12">
-        <v>44</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>25</v>
-      </c>
-      <c r="J12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>50</v>
-      </c>
-      <c r="E13">
-        <v>44</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>25</v>
-      </c>
-      <c r="J13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>378</v>
-      </c>
-      <c r="C14" t="s">
-        <v>378</v>
-      </c>
-      <c r="D14">
-        <v>810</v>
-      </c>
-      <c r="E14">
-        <v>800</v>
-      </c>
-      <c r="F14">
-        <v>3020</v>
-      </c>
-      <c r="G14">
-        <v>622</v>
-      </c>
-      <c r="H14">
-        <v>1200</v>
-      </c>
-      <c r="I14">
-        <v>630</v>
-      </c>
-      <c r="J14">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>378</v>
-      </c>
-      <c r="C15" t="s">
-        <v>378</v>
-      </c>
-      <c r="D15">
-        <v>13</v>
-      </c>
-      <c r="E15">
-        <v>10</v>
-      </c>
-      <c r="F15">
-        <v>13</v>
-      </c>
-      <c r="G15">
-        <v>12</v>
-      </c>
-      <c r="H15">
-        <v>72</v>
-      </c>
-      <c r="I15">
-        <v>12</v>
-      </c>
-      <c r="J15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>378</v>
-      </c>
-      <c r="C16" t="s">
-        <v>378</v>
-      </c>
-      <c r="D16">
-        <v>50</v>
-      </c>
-      <c r="E16">
-        <v>44</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>25</v>
-      </c>
-      <c r="J16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>378</v>
-      </c>
-      <c r="C17" t="s">
-        <v>378</v>
-      </c>
-      <c r="D17">
-        <v>50</v>
-      </c>
-      <c r="E17">
-        <v>44</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>25</v>
-      </c>
-      <c r="J17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>810</v>
-      </c>
-      <c r="E18">
-        <v>800</v>
-      </c>
-      <c r="F18">
-        <v>3020</v>
-      </c>
-      <c r="G18">
-        <v>622</v>
-      </c>
-      <c r="H18">
-        <v>1200</v>
-      </c>
-      <c r="I18">
-        <v>630</v>
-      </c>
-      <c r="J18">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>13</v>
-      </c>
-      <c r="E19">
-        <v>10</v>
-      </c>
-      <c r="F19">
-        <v>13</v>
-      </c>
-      <c r="G19">
-        <v>12</v>
-      </c>
-      <c r="H19">
-        <v>72</v>
-      </c>
-      <c r="I19">
-        <v>12</v>
-      </c>
-      <c r="J19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>50</v>
-      </c>
-      <c r="E20">
-        <v>44</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>25</v>
-      </c>
-      <c r="J20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>50</v>
-      </c>
-      <c r="E21">
-        <v>44</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>25</v>
-      </c>
-      <c r="J21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s">
-        <v>378</v>
-      </c>
-      <c r="C22" t="s">
-        <v>378</v>
-      </c>
-      <c r="D22">
-        <v>810</v>
-      </c>
-      <c r="E22">
-        <v>800</v>
-      </c>
-      <c r="F22">
-        <v>3020</v>
-      </c>
-      <c r="G22">
-        <v>622</v>
-      </c>
-      <c r="H22">
-        <v>1200</v>
-      </c>
-      <c r="I22">
-        <v>630</v>
-      </c>
-      <c r="J22">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23">
-        <v>0</v>
-      </c>
-      <c r="B23" t="s">
-        <v>378</v>
-      </c>
-      <c r="C23" t="s">
-        <v>378</v>
-      </c>
-      <c r="D23">
-        <v>13</v>
-      </c>
-      <c r="E23">
-        <v>10</v>
-      </c>
-      <c r="F23">
-        <v>13</v>
-      </c>
-      <c r="G23">
-        <v>12</v>
-      </c>
-      <c r="H23">
-        <v>72</v>
-      </c>
-      <c r="I23">
-        <v>12</v>
-      </c>
-      <c r="J23">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24">
-        <v>0</v>
-      </c>
-      <c r="B24" t="s">
-        <v>378</v>
-      </c>
-      <c r="C24" t="s">
-        <v>378</v>
-      </c>
-      <c r="D24">
-        <v>50</v>
-      </c>
-      <c r="E24">
-        <v>44</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>25</v>
-      </c>
-      <c r="J24">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25">
-        <v>0</v>
-      </c>
-      <c r="B25" t="s">
-        <v>378</v>
-      </c>
-      <c r="C25" t="s">
-        <v>378</v>
-      </c>
-      <c r="D25">
-        <v>50</v>
-      </c>
-      <c r="E25">
-        <v>44</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <v>25</v>
-      </c>
-      <c r="J25">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>810</v>
-      </c>
-      <c r="E26">
-        <v>800</v>
-      </c>
-      <c r="F26">
-        <v>3020</v>
-      </c>
-      <c r="G26">
-        <v>622</v>
-      </c>
-      <c r="H26">
-        <v>1200</v>
-      </c>
-      <c r="I26">
-        <v>630</v>
-      </c>
-      <c r="J26">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27">
-        <v>0</v>
-      </c>
-      <c r="D27">
-        <v>13</v>
-      </c>
-      <c r="E27">
-        <v>10</v>
-      </c>
-      <c r="F27">
-        <v>13</v>
-      </c>
-      <c r="G27">
-        <v>12</v>
-      </c>
-      <c r="H27">
-        <v>72</v>
-      </c>
-      <c r="I27">
-        <v>12</v>
-      </c>
-      <c r="J27">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>50</v>
-      </c>
-      <c r="E28">
-        <v>44</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>25</v>
-      </c>
-      <c r="J28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29">
-        <v>0</v>
-      </c>
-      <c r="D29">
-        <v>50</v>
-      </c>
-      <c r="E29">
-        <v>44</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <v>25</v>
-      </c>
-      <c r="J29">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30">
-        <v>0</v>
-      </c>
-      <c r="B30" t="s">
-        <v>378</v>
-      </c>
-      <c r="C30" t="s">
-        <v>378</v>
-      </c>
-      <c r="D30">
-        <v>810</v>
-      </c>
-      <c r="E30">
-        <v>800</v>
-      </c>
-      <c r="F30">
-        <v>3020</v>
-      </c>
-      <c r="G30">
-        <v>622</v>
-      </c>
-      <c r="H30">
-        <v>1200</v>
-      </c>
-      <c r="I30">
-        <v>630</v>
-      </c>
-      <c r="J30">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31">
-        <v>0</v>
-      </c>
-      <c r="B31" t="s">
-        <v>378</v>
-      </c>
-      <c r="C31" t="s">
-        <v>378</v>
-      </c>
-      <c r="D31">
-        <v>13</v>
-      </c>
-      <c r="E31">
-        <v>10</v>
-      </c>
-      <c r="F31">
-        <v>13</v>
-      </c>
-      <c r="G31">
-        <v>12</v>
-      </c>
-      <c r="H31">
-        <v>72</v>
-      </c>
-      <c r="I31">
-        <v>12</v>
-      </c>
-      <c r="J31">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32">
-        <v>0</v>
-      </c>
-      <c r="B32" t="s">
-        <v>378</v>
-      </c>
-      <c r="C32" t="s">
-        <v>378</v>
-      </c>
-      <c r="D32">
-        <v>50</v>
-      </c>
-      <c r="E32">
-        <v>44</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>25</v>
-      </c>
-      <c r="J32">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33">
-        <v>0</v>
-      </c>
-      <c r="B33" t="s">
-        <v>378</v>
-      </c>
-      <c r="C33" t="s">
-        <v>378</v>
-      </c>
-      <c r="D33">
-        <v>50</v>
-      </c>
-      <c r="E33">
-        <v>44</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
-      </c>
-      <c r="I33">
-        <v>25</v>
-      </c>
-      <c r="J33">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34">
-        <v>0</v>
-      </c>
-      <c r="D34">
-        <v>810</v>
-      </c>
-      <c r="E34">
-        <v>800</v>
-      </c>
-      <c r="F34">
-        <v>3020</v>
-      </c>
-      <c r="G34">
-        <v>622</v>
-      </c>
-      <c r="H34">
-        <v>1200</v>
-      </c>
-      <c r="I34">
-        <v>630</v>
-      </c>
-      <c r="J34">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35">
-        <v>0</v>
-      </c>
-      <c r="D35">
-        <v>13</v>
-      </c>
-      <c r="E35">
-        <v>10</v>
-      </c>
-      <c r="F35">
-        <v>13</v>
-      </c>
-      <c r="G35">
-        <v>12</v>
-      </c>
-      <c r="H35">
-        <v>72</v>
-      </c>
-      <c r="I35">
-        <v>12</v>
-      </c>
-      <c r="J35">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>50</v>
-      </c>
-      <c r="E36">
-        <v>44</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-      <c r="G36">
-        <v>0</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-      <c r="I36">
-        <v>25</v>
-      </c>
-      <c r="J36">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>50</v>
-      </c>
-      <c r="E37">
-        <v>44</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>25</v>
-      </c>
-      <c r="J37">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38">
-        <v>0</v>
-      </c>
-      <c r="B38" t="s">
-        <v>378</v>
-      </c>
-      <c r="C38" t="s">
-        <v>378</v>
-      </c>
-      <c r="D38">
-        <v>810</v>
-      </c>
-      <c r="E38">
-        <v>800</v>
-      </c>
-      <c r="F38">
-        <v>3020</v>
-      </c>
-      <c r="G38">
-        <v>622</v>
-      </c>
-      <c r="H38">
-        <v>1200</v>
-      </c>
-      <c r="I38">
-        <v>630</v>
-      </c>
-      <c r="J38">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39">
-        <v>0</v>
-      </c>
-      <c r="B39" t="s">
-        <v>378</v>
-      </c>
-      <c r="C39" t="s">
-        <v>378</v>
-      </c>
-      <c r="D39">
-        <v>13</v>
-      </c>
-      <c r="E39">
-        <v>10</v>
-      </c>
-      <c r="F39">
-        <v>13</v>
-      </c>
-      <c r="G39">
-        <v>12</v>
-      </c>
-      <c r="H39">
-        <v>72</v>
-      </c>
-      <c r="I39">
-        <v>12</v>
-      </c>
-      <c r="J39">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40">
-        <v>0</v>
-      </c>
-      <c r="B40" t="s">
-        <v>378</v>
-      </c>
-      <c r="C40" t="s">
-        <v>378</v>
-      </c>
-      <c r="D40">
-        <v>50</v>
-      </c>
-      <c r="E40">
-        <v>44</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>25</v>
-      </c>
-      <c r="J40">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41">
-        <v>0</v>
-      </c>
-      <c r="B41" t="s">
-        <v>378</v>
-      </c>
-      <c r="C41" t="s">
-        <v>378</v>
-      </c>
-      <c r="D41">
-        <v>50</v>
-      </c>
-      <c r="E41">
-        <v>44</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>25</v>
-      </c>
-      <c r="J41">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>378</v>
-      </c>
-      <c r="C2">
-        <v>800</v>
-      </c>
-      <c r="D2">
-        <v>3020</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>378</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>378</v>
-      </c>
-      <c r="C4">
-        <v>44</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>378</v>
-      </c>
-      <c r="C5">
-        <v>44</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>378</v>
-      </c>
-      <c r="C6">
-        <v>800</v>
-      </c>
-      <c r="D6">
-        <v>3020</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>378</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>378</v>
-      </c>
-      <c r="C8">
-        <v>44</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>378</v>
-      </c>
-      <c r="C9">
-        <v>44</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>378</v>
-      </c>
-      <c r="C10">
-        <v>800</v>
-      </c>
-      <c r="D10">
-        <v>3020</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>378</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>378</v>
-      </c>
-      <c r="C12">
-        <v>44</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>378</v>
-      </c>
-      <c r="C13">
-        <v>44</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>378</v>
-      </c>
-      <c r="C14">
-        <v>800</v>
-      </c>
-      <c r="D14">
-        <v>3020</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>378</v>
-      </c>
-      <c r="C15">
-        <v>10</v>
-      </c>
-      <c r="D15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>378</v>
-      </c>
-      <c r="C16">
-        <v>44</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>378</v>
-      </c>
-      <c r="C17">
-        <v>44</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="B18" t="s">
-        <v>378</v>
-      </c>
-      <c r="C18">
-        <v>800</v>
-      </c>
-      <c r="D18">
-        <v>3020</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19" t="s">
-        <v>378</v>
-      </c>
-      <c r="C19">
-        <v>10</v>
-      </c>
-      <c r="D19">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>378</v>
-      </c>
-      <c r="C20">
-        <v>44</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>378</v>
-      </c>
-      <c r="C21">
-        <v>44</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
-        <v>0</v>
-      </c>
-      <c r="B22" t="s">
-        <v>378</v>
-      </c>
-      <c r="C22">
-        <v>800</v>
-      </c>
-      <c r="D22">
-        <v>3020</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23">
-        <v>0</v>
-      </c>
-      <c r="B23" t="s">
-        <v>378</v>
-      </c>
-      <c r="C23">
-        <v>10</v>
-      </c>
-      <c r="D23">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24">
-        <v>0</v>
-      </c>
-      <c r="B24" t="s">
-        <v>378</v>
-      </c>
-      <c r="C24">
-        <v>44</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25">
-        <v>0</v>
-      </c>
-      <c r="B25" t="s">
-        <v>378</v>
-      </c>
-      <c r="C25">
-        <v>44</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>378</v>
-      </c>
-      <c r="C8" t="s">
-        <v>378</v>
-      </c>
-      <c r="D8">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>378</v>
-      </c>
-      <c r="C9" t="s">
-        <v>378</v>
-      </c>
-      <c r="D9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>378</v>
-      </c>
-      <c r="C12" t="s">
-        <v>378</v>
-      </c>
-      <c r="D12">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>378</v>
-      </c>
-      <c r="C13" t="s">
-        <v>378</v>
-      </c>
-      <c r="D13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>378</v>
-      </c>
-      <c r="C16" t="s">
-        <v>378</v>
-      </c>
-      <c r="D16">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>378</v>
-      </c>
-      <c r="C17" t="s">
-        <v>378</v>
-      </c>
-      <c r="D17">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>378</v>
-      </c>
-      <c r="C20" t="s">
-        <v>378</v>
-      </c>
-      <c r="D20">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>378</v>
-      </c>
-      <c r="C21" t="s">
-        <v>378</v>
-      </c>
-      <c r="D21">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>378</v>
-      </c>
-      <c r="C8" t="s">
-        <v>378</v>
-      </c>
-      <c r="D8">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>378</v>
-      </c>
-      <c r="C9" t="s">
-        <v>378</v>
-      </c>
-      <c r="D9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>378</v>
-      </c>
-      <c r="C12" t="s">
-        <v>378</v>
-      </c>
-      <c r="D12">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>378</v>
-      </c>
-      <c r="C13" t="s">
-        <v>378</v>
-      </c>
-      <c r="D13">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>378</v>
-      </c>
-      <c r="C16" t="s">
-        <v>378</v>
-      </c>
-      <c r="D16">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>378</v>
-      </c>
-      <c r="C17" t="s">
-        <v>378</v>
-      </c>
-      <c r="D17">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>378</v>
-      </c>
-      <c r="C20" t="s">
-        <v>378</v>
-      </c>
-      <c r="D20">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>378</v>
-      </c>
-      <c r="C21" t="s">
-        <v>378</v>
-      </c>
-      <c r="D21">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>378</v>
-      </c>
-      <c r="C8" t="s">
-        <v>378</v>
-      </c>
-      <c r="D8">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>378</v>
-      </c>
-      <c r="C9" t="s">
-        <v>378</v>
-      </c>
-      <c r="D9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
-        <v>378</v>
-      </c>
-      <c r="C12" t="s">
-        <v>378</v>
-      </c>
-      <c r="D12">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>378</v>
-      </c>
-      <c r="C13" t="s">
-        <v>378</v>
-      </c>
-      <c r="D13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>378</v>
-      </c>
-      <c r="C16" t="s">
-        <v>378</v>
-      </c>
-      <c r="D16">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17" t="s">
-        <v>378</v>
-      </c>
-      <c r="C17" t="s">
-        <v>378</v>
-      </c>
-      <c r="D17">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20" t="s">
-        <v>378</v>
-      </c>
-      <c r="C20" t="s">
-        <v>378</v>
-      </c>
-      <c r="D20">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>378</v>
-      </c>
-      <c r="C21" t="s">
-        <v>378</v>
-      </c>
-      <c r="D21">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F122"/>

</xml_diff>